<commit_message>
0.0.16: Support [] (means empty array) on JSON.
</commit_message>
<xml_diff>
--- a/meta/test2/04_GetTableSample5.xlsx
+++ b/meta/test2/04_GetTableSample5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/test2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C58746-5221-9B45-B203-94DE031390C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D58D757-3ACA-974B-A9B5-1C606EED4283}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11240" yWindow="2500" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="130">
   <si>
     <t>2.定義書様式に記入された情報から、メタファイルをXMLファイルに変換する処理の定義に相当するJavaソースコードが自動生成されます。</t>
   </si>
@@ -703,6 +703,17 @@
   <si>
     <t>JSON</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>JSON指定なし</t>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="12"/>
   </si>
 </sst>
 </file>
@@ -879,7 +890,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="97">
+  <borders count="96">
     <border>
       <left/>
       <right/>
@@ -1687,19 +1698,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
       <bottom style="hair">
         <color auto="1"/>
       </bottom>
@@ -2119,7 +2117,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2450,16 +2448,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2495,7 +2490,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2510,7 +2505,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2519,16 +2517,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2546,7 +2541,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2555,7 +2550,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2569,40 +2564,43 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="73" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="78" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="76" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="80" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="72" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="77" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="75" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="79" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2614,7 +2612,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="86" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2623,43 +2621,40 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="87" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="88" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="75" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="89" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="90" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2671,28 +2666,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2707,26 +2708,20 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -3050,7 +3045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B86D5CC-26D4-0349-B89F-A4BFBE2080C4}">
   <dimension ref="A1:W1044"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -3167,11 +3162,11 @@
         <v>31</v>
       </c>
       <c r="B9" s="88"/>
-      <c r="C9" s="158" t="s">
+      <c r="C9" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
+      <c r="D9" s="158"/>
+      <c r="E9" s="158"/>
       <c r="F9" s="91"/>
       <c r="G9" s="92"/>
       <c r="H9" s="75"/>
@@ -3293,33 +3288,33 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A19" s="136"/>
-      <c r="B19" s="137"/>
-      <c r="C19" s="137"/>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137"/>
-      <c r="G19" s="137"/>
-      <c r="H19" s="137"/>
-      <c r="I19" s="137"/>
-      <c r="J19" s="137"/>
-      <c r="K19" s="137"/>
-      <c r="L19" s="138"/>
-      <c r="M19" s="205" t="s">
+      <c r="A19" s="135"/>
+      <c r="B19" s="136"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="136"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="136"/>
+      <c r="G19" s="136"/>
+      <c r="H19" s="136"/>
+      <c r="I19" s="136"/>
+      <c r="J19" s="136"/>
+      <c r="K19" s="136"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="206" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="206"/>
-      <c r="O19" s="206"/>
-      <c r="P19" s="206"/>
-      <c r="Q19" s="206"/>
-      <c r="R19" s="205" t="s">
+      <c r="N19" s="207"/>
+      <c r="O19" s="207"/>
+      <c r="P19" s="207"/>
+      <c r="Q19" s="207"/>
+      <c r="R19" s="206" t="s">
         <v>43</v>
       </c>
-      <c r="S19" s="206"/>
-      <c r="T19" s="206"/>
-      <c r="U19" s="206"/>
-      <c r="V19" s="206"/>
-      <c r="W19" s="139"/>
+      <c r="S19" s="207"/>
+      <c r="T19" s="207"/>
+      <c r="U19" s="207"/>
+      <c r="V19" s="207"/>
+      <c r="W19" s="138"/>
     </row>
     <row r="20" spans="1:23" ht="12.75" customHeight="1">
       <c r="A20" s="114"/>
@@ -3335,91 +3330,91 @@
       <c r="I20" s="114"/>
       <c r="J20" s="114"/>
       <c r="K20" s="114"/>
-      <c r="L20" s="140"/>
-      <c r="M20" s="203" t="s">
+      <c r="L20" s="139"/>
+      <c r="M20" s="204" t="s">
         <v>65</v>
       </c>
-      <c r="N20" s="204"/>
-      <c r="O20" s="204"/>
-      <c r="P20" s="204"/>
-      <c r="Q20" s="204"/>
-      <c r="R20" s="203" t="s">
+      <c r="N20" s="205"/>
+      <c r="O20" s="205"/>
+      <c r="P20" s="205"/>
+      <c r="Q20" s="205"/>
+      <c r="R20" s="204" t="s">
         <v>65</v>
       </c>
-      <c r="S20" s="204"/>
-      <c r="T20" s="204"/>
-      <c r="U20" s="204"/>
-      <c r="V20" s="204"/>
+      <c r="S20" s="205"/>
+      <c r="T20" s="205"/>
+      <c r="U20" s="205"/>
+      <c r="V20" s="205"/>
       <c r="W20" s="114"/>
     </row>
     <row r="21" spans="1:23" ht="23" customHeight="1">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="157" t="s">
+      <c r="C21" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="157" t="s">
+      <c r="D21" s="156" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="156" t="s">
+      <c r="E21" s="155" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="156" t="s">
+      <c r="F21" s="155" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="156" t="s">
+      <c r="G21" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="156" t="s">
+      <c r="H21" s="155" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="156" t="s">
+      <c r="I21" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="156" t="s">
+      <c r="J21" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="156" t="s">
+      <c r="K21" s="155" t="s">
         <v>53</v>
       </c>
-      <c r="L21" s="160" t="s">
+      <c r="L21" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="M21" s="156" t="s">
+      <c r="M21" s="155" t="s">
         <v>66</v>
       </c>
-      <c r="N21" s="156" t="s">
+      <c r="N21" s="155" t="s">
         <v>67</v>
       </c>
-      <c r="O21" s="156" t="s">
+      <c r="O21" s="155" t="s">
         <v>68</v>
       </c>
-      <c r="P21" s="156" t="s">
+      <c r="P21" s="155" t="s">
         <v>69</v>
       </c>
-      <c r="Q21" s="156" t="s">
+      <c r="Q21" s="155" t="s">
         <v>70</v>
       </c>
-      <c r="R21" s="156" t="s">
+      <c r="R21" s="155" t="s">
         <v>71</v>
       </c>
-      <c r="S21" s="156" t="s">
+      <c r="S21" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="T21" s="156" t="s">
+      <c r="T21" s="155" t="s">
         <v>73</v>
       </c>
-      <c r="U21" s="156" t="s">
+      <c r="U21" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="V21" s="156" t="s">
+      <c r="V21" s="155" t="s">
         <v>75</v>
       </c>
-      <c r="W21" s="156" t="s">
+      <c r="W21" s="155" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3431,7 +3426,7 @@
         <v>32</v>
       </c>
       <c r="C22" s="16"/>
-      <c r="D22" s="145" t="s">
+      <c r="D22" s="144" t="s">
         <v>89</v>
       </c>
       <c r="E22" s="16" t="s">
@@ -3445,29 +3440,29 @@
       <c r="I22" s="117"/>
       <c r="J22" s="117"/>
       <c r="K22" s="117"/>
-      <c r="L22" s="148">
+      <c r="L22" s="147">
         <v>1</v>
       </c>
-      <c r="M22" s="149"/>
-      <c r="N22" s="150"/>
-      <c r="O22" s="151" t="s">
+      <c r="M22" s="148"/>
+      <c r="N22" s="149"/>
+      <c r="O22" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="151" t="s">
+      <c r="P22" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="Q22" s="149" t="s">
+      <c r="Q22" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="R22" s="149"/>
-      <c r="S22" s="150"/>
-      <c r="T22" s="151" t="s">
+      <c r="R22" s="148"/>
+      <c r="S22" s="149"/>
+      <c r="T22" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="U22" s="151" t="s">
+      <c r="U22" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="V22" s="149" t="s">
+      <c r="V22" s="148" t="s">
         <v>39</v>
       </c>
       <c r="W22" s="35"/>
@@ -3480,7 +3475,7 @@
         <v>104</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="145" t="s">
+      <c r="D23" s="144" t="s">
         <v>89</v>
       </c>
       <c r="E23" s="16" t="s">
@@ -3494,29 +3489,29 @@
       <c r="I23" s="117"/>
       <c r="J23" s="117"/>
       <c r="K23" s="117"/>
-      <c r="L23" s="148">
+      <c r="L23" s="147">
         <v>2</v>
       </c>
-      <c r="M23" s="149"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="151" t="s">
+      <c r="M23" s="148"/>
+      <c r="N23" s="149"/>
+      <c r="O23" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="P23" s="151" t="s">
+      <c r="P23" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="Q23" s="149" t="s">
+      <c r="Q23" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="R23" s="149"/>
-      <c r="S23" s="150"/>
-      <c r="T23" s="151" t="s">
+      <c r="R23" s="148"/>
+      <c r="S23" s="149"/>
+      <c r="T23" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="U23" s="151" t="s">
+      <c r="U23" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="V23" s="149" t="s">
+      <c r="V23" s="148" t="s">
         <v>39</v>
       </c>
       <c r="W23" s="16"/>
@@ -3529,7 +3524,7 @@
         <v>105</v>
       </c>
       <c r="C24" s="16"/>
-      <c r="D24" s="145" t="s">
+      <c r="D24" s="144" t="s">
         <v>89</v>
       </c>
       <c r="E24" s="16" t="s">
@@ -3543,88 +3538,112 @@
       <c r="I24" s="117"/>
       <c r="J24" s="117"/>
       <c r="K24" s="117"/>
-      <c r="L24" s="148">
+      <c r="L24" s="147">
         <v>3</v>
       </c>
-      <c r="M24" s="149"/>
-      <c r="N24" s="150"/>
-      <c r="O24" s="151" t="s">
+      <c r="M24" s="148"/>
+      <c r="N24" s="149"/>
+      <c r="O24" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="P24" s="151" t="s">
+      <c r="P24" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="Q24" s="149" t="s">
+      <c r="Q24" s="148" t="s">
         <v>39</v>
       </c>
-      <c r="R24" s="149"/>
-      <c r="S24" s="150"/>
-      <c r="T24" s="151" t="s">
+      <c r="R24" s="148"/>
+      <c r="S24" s="149"/>
+      <c r="T24" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="U24" s="151" t="s">
+      <c r="U24" s="150" t="s">
         <v>38</v>
       </c>
-      <c r="V24" s="149" t="s">
+      <c r="V24" s="148" t="s">
         <v>39</v>
       </c>
       <c r="W24" s="16"/>
     </row>
     <row r="25" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A25" s="16"/>
-      <c r="B25" s="141"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="146"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="125"/>
-      <c r="N25" s="130"/>
-      <c r="O25" s="132"/>
-      <c r="P25" s="134"/>
-      <c r="Q25" s="125"/>
-      <c r="R25" s="125"/>
-      <c r="S25" s="130"/>
-      <c r="T25" s="132"/>
-      <c r="U25" s="134"/>
-      <c r="V25" s="125"/>
+      <c r="A25" s="35">
+        <v>4</v>
+      </c>
+      <c r="B25" s="95" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="144" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="119" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="117"/>
+      <c r="H25" s="117"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="117"/>
+      <c r="K25" s="117"/>
+      <c r="L25" s="147">
+        <v>4</v>
+      </c>
+      <c r="M25" s="148"/>
+      <c r="N25" s="149"/>
+      <c r="O25" s="150" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25" s="150" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="148" t="s">
+        <v>39</v>
+      </c>
+      <c r="R25" s="148"/>
+      <c r="S25" s="149"/>
+      <c r="T25" s="150" t="s">
+        <v>37</v>
+      </c>
+      <c r="U25" s="150" t="s">
+        <v>38</v>
+      </c>
+      <c r="V25" s="148" t="s">
+        <v>39</v>
+      </c>
       <c r="W25" s="95"/>
     </row>
     <row r="26" spans="1:23" ht="12.75" customHeight="1">
       <c r="A26" s="11"/>
-      <c r="B26" s="141"/>
+      <c r="B26" s="140"/>
       <c r="C26" s="11"/>
-      <c r="D26" s="146"/>
+      <c r="D26" s="145"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="147"/>
+      <c r="F26" s="146"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
-      <c r="M26" s="125"/>
-      <c r="N26" s="130"/>
-      <c r="O26" s="133"/>
-      <c r="P26" s="135"/>
-      <c r="Q26" s="125"/>
-      <c r="R26" s="125"/>
-      <c r="S26" s="130"/>
-      <c r="T26" s="133"/>
-      <c r="U26" s="135"/>
-      <c r="V26" s="125"/>
-      <c r="W26" s="153"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="129"/>
+      <c r="O26" s="132"/>
+      <c r="P26" s="134"/>
+      <c r="Q26" s="124"/>
+      <c r="R26" s="124"/>
+      <c r="S26" s="129"/>
+      <c r="T26" s="132"/>
+      <c r="U26" s="134"/>
+      <c r="V26" s="124"/>
+      <c r="W26" s="152"/>
     </row>
     <row r="27" spans="1:23" ht="12.75" customHeight="1">
       <c r="A27" s="14"/>
-      <c r="B27" s="142"/>
+      <c r="B27" s="141"/>
       <c r="C27" s="14"/>
-      <c r="D27" s="142"/>
+      <c r="D27" s="141"/>
       <c r="E27" s="14"/>
       <c r="F27" s="119"/>
       <c r="G27" s="14"/>
@@ -3633,23 +3652,23 @@
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
       <c r="L27" s="14"/>
-      <c r="M27" s="126"/>
-      <c r="N27" s="128"/>
-      <c r="O27" s="131"/>
-      <c r="P27" s="131"/>
-      <c r="Q27" s="124"/>
-      <c r="R27" s="126"/>
-      <c r="S27" s="128"/>
-      <c r="T27" s="131"/>
-      <c r="U27" s="131"/>
-      <c r="V27" s="124"/>
+      <c r="M27" s="125"/>
+      <c r="N27" s="127"/>
+      <c r="O27" s="130"/>
+      <c r="P27" s="130"/>
+      <c r="Q27" s="123"/>
+      <c r="R27" s="125"/>
+      <c r="S27" s="127"/>
+      <c r="T27" s="130"/>
+      <c r="U27" s="130"/>
+      <c r="V27" s="123"/>
       <c r="W27" s="35"/>
     </row>
     <row r="28" spans="1:23" ht="12.75" customHeight="1">
       <c r="A28" s="16"/>
-      <c r="B28" s="143"/>
+      <c r="B28" s="142"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="143"/>
+      <c r="D28" s="142"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
@@ -3658,23 +3677,23 @@
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
       <c r="L28" s="16"/>
-      <c r="M28" s="125"/>
-      <c r="N28" s="129"/>
-      <c r="O28" s="132"/>
-      <c r="P28" s="134"/>
-      <c r="Q28" s="125"/>
-      <c r="R28" s="125"/>
-      <c r="S28" s="129"/>
-      <c r="T28" s="132"/>
-      <c r="U28" s="134"/>
-      <c r="V28" s="125"/>
+      <c r="M28" s="124"/>
+      <c r="N28" s="128"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="133"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="128"/>
+      <c r="T28" s="131"/>
+      <c r="U28" s="133"/>
+      <c r="V28" s="124"/>
       <c r="W28" s="16"/>
     </row>
     <row r="29" spans="1:23" ht="12.75" customHeight="1">
       <c r="A29" s="16"/>
-      <c r="B29" s="143"/>
+      <c r="B29" s="142"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="145"/>
+      <c r="D29" s="144"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
@@ -3683,23 +3702,23 @@
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
       <c r="L29" s="16"/>
-      <c r="M29" s="125"/>
-      <c r="N29" s="129"/>
-      <c r="O29" s="132"/>
-      <c r="P29" s="134"/>
-      <c r="Q29" s="125"/>
-      <c r="R29" s="125"/>
-      <c r="S29" s="129"/>
-      <c r="T29" s="132"/>
-      <c r="U29" s="134"/>
-      <c r="V29" s="125"/>
+      <c r="M29" s="124"/>
+      <c r="N29" s="128"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="133"/>
+      <c r="Q29" s="124"/>
+      <c r="R29" s="124"/>
+      <c r="S29" s="128"/>
+      <c r="T29" s="131"/>
+      <c r="U29" s="133"/>
+      <c r="V29" s="124"/>
       <c r="W29" s="95"/>
     </row>
     <row r="30" spans="1:23" ht="12.75" customHeight="1">
       <c r="A30" s="16"/>
-      <c r="B30" s="143"/>
+      <c r="B30" s="142"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="143"/>
+      <c r="D30" s="142"/>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -3708,48 +3727,48 @@
       <c r="J30" s="20"/>
       <c r="K30" s="20"/>
       <c r="L30" s="16"/>
-      <c r="M30" s="125"/>
-      <c r="N30" s="130"/>
-      <c r="O30" s="132"/>
-      <c r="P30" s="134"/>
-      <c r="Q30" s="125"/>
-      <c r="R30" s="125"/>
-      <c r="S30" s="130"/>
-      <c r="T30" s="132"/>
-      <c r="U30" s="134"/>
-      <c r="V30" s="125"/>
-      <c r="W30" s="155"/>
+      <c r="M30" s="124"/>
+      <c r="N30" s="129"/>
+      <c r="O30" s="131"/>
+      <c r="P30" s="133"/>
+      <c r="Q30" s="124"/>
+      <c r="R30" s="124"/>
+      <c r="S30" s="129"/>
+      <c r="T30" s="131"/>
+      <c r="U30" s="133"/>
+      <c r="V30" s="124"/>
+      <c r="W30" s="154"/>
     </row>
     <row r="31" spans="1:23" ht="12.75" customHeight="1">
       <c r="A31" s="11"/>
-      <c r="B31" s="141"/>
+      <c r="B31" s="140"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="146"/>
+      <c r="D31" s="145"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="121"/>
+      <c r="F31" s="120"/>
       <c r="G31" s="11"/>
       <c r="H31" s="118"/>
       <c r="I31" s="118"/>
       <c r="J31" s="118"/>
       <c r="K31" s="118"/>
       <c r="L31" s="11"/>
-      <c r="M31" s="125"/>
-      <c r="N31" s="130"/>
-      <c r="O31" s="133"/>
-      <c r="P31" s="135"/>
-      <c r="Q31" s="125"/>
-      <c r="R31" s="125"/>
-      <c r="S31" s="130"/>
-      <c r="T31" s="133"/>
-      <c r="U31" s="135"/>
-      <c r="V31" s="125"/>
-      <c r="W31" s="154"/>
+      <c r="M31" s="124"/>
+      <c r="N31" s="129"/>
+      <c r="O31" s="132"/>
+      <c r="P31" s="134"/>
+      <c r="Q31" s="124"/>
+      <c r="R31" s="124"/>
+      <c r="S31" s="129"/>
+      <c r="T31" s="132"/>
+      <c r="U31" s="134"/>
+      <c r="V31" s="124"/>
+      <c r="W31" s="153"/>
     </row>
     <row r="32" spans="1:23" ht="12.75" customHeight="1">
       <c r="A32" s="14"/>
       <c r="B32" s="94"/>
       <c r="C32" s="14"/>
-      <c r="D32" s="144"/>
+      <c r="D32" s="143"/>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
@@ -3758,16 +3777,16 @@
       <c r="J32" s="14"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
-      <c r="M32" s="127"/>
-      <c r="N32" s="128"/>
-      <c r="O32" s="131"/>
-      <c r="P32" s="131"/>
-      <c r="Q32" s="124"/>
-      <c r="R32" s="127"/>
-      <c r="S32" s="128"/>
-      <c r="T32" s="131"/>
-      <c r="U32" s="131"/>
-      <c r="V32" s="124"/>
+      <c r="M32" s="126"/>
+      <c r="N32" s="127"/>
+      <c r="O32" s="130"/>
+      <c r="P32" s="130"/>
+      <c r="Q32" s="123"/>
+      <c r="R32" s="126"/>
+      <c r="S32" s="127"/>
+      <c r="T32" s="130"/>
+      <c r="U32" s="130"/>
+      <c r="V32" s="123"/>
     </row>
     <row r="33" spans="1:23" ht="12.75" customHeight="1">
       <c r="A33" s="16"/>
@@ -4250,7 +4269,7 @@
       <c r="C52" s="110"/>
       <c r="D52" s="110"/>
       <c r="E52" s="109"/>
-      <c r="F52" s="122"/>
+      <c r="F52" s="121"/>
       <c r="G52" s="109"/>
       <c r="H52" s="109"/>
       <c r="I52" s="109"/>
@@ -4375,7 +4394,7 @@
       <c r="C57" s="110"/>
       <c r="D57" s="110"/>
       <c r="E57" s="109"/>
-      <c r="F57" s="122"/>
+      <c r="F57" s="121"/>
       <c r="G57" s="109"/>
       <c r="H57" s="109"/>
       <c r="I57" s="109"/>
@@ -4500,7 +4519,7 @@
       <c r="C62" s="58"/>
       <c r="D62" s="58"/>
       <c r="E62" s="57"/>
-      <c r="F62" s="123"/>
+      <c r="F62" s="122"/>
       <c r="G62" s="57"/>
       <c r="H62" s="57"/>
       <c r="I62" s="57"/>
@@ -4625,7 +4644,7 @@
       <c r="C67" s="58"/>
       <c r="D67" s="58"/>
       <c r="E67" s="57"/>
-      <c r="F67" s="123"/>
+      <c r="F67" s="122"/>
       <c r="G67" s="57"/>
       <c r="H67" s="57"/>
       <c r="I67" s="57"/>
@@ -4750,7 +4769,7 @@
       <c r="C72" s="58"/>
       <c r="D72" s="58"/>
       <c r="E72" s="57"/>
-      <c r="F72" s="123"/>
+      <c r="F72" s="122"/>
       <c r="G72" s="57"/>
       <c r="H72" s="57"/>
       <c r="I72" s="57"/>
@@ -5835,10 +5854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2255131-13B1-484A-9393-AFEFC966B3D8}">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -5878,7 +5897,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="197"/>
+      <c r="E3" s="196"/>
       <c r="F3" s="75"/>
       <c r="G3" s="75"/>
       <c r="H3" s="75"/>
@@ -5897,7 +5916,7 @@
         <v>90</v>
       </c>
       <c r="D4" s="8"/>
-      <c r="E4" s="198"/>
+      <c r="E4" s="197"/>
       <c r="F4" s="75"/>
       <c r="G4" s="75"/>
       <c r="H4" s="75"/>
@@ -5915,8 +5934,8 @@
       <c r="C5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="196"/>
-      <c r="E5" s="199"/>
+      <c r="D5" s="195"/>
+      <c r="E5" s="198"/>
       <c r="F5" s="75"/>
       <c r="G5" s="75"/>
       <c r="H5" s="75"/>
@@ -5935,7 +5954,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="198"/>
+      <c r="E6" s="197"/>
       <c r="F6" s="75"/>
       <c r="G6" s="75"/>
       <c r="H6" s="75"/>
@@ -5978,7 +5997,7 @@
         <v>82</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="152"/>
+      <c r="C11" s="151"/>
       <c r="D11" s="10">
         <v>1</v>
       </c>
@@ -6022,11 +6041,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="165" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A12" s="173" t="s">
+    <row r="12" spans="1:17" s="164" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A12" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="174" t="s">
+      <c r="B12" s="173" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="80" t="s">
@@ -6060,7 +6079,7 @@
         <f t="shared" si="0"/>
         <v>Input7</v>
       </c>
-      <c r="K12" s="175" t="str">
+      <c r="K12" s="174" t="str">
         <f>"Expect"&amp;K11</f>
         <v>Expect1</v>
       </c>
@@ -6068,322 +6087,322 @@
         <f t="shared" ref="L12:M12" si="1">"Expect"&amp;L11</f>
         <v>Expect2</v>
       </c>
-      <c r="M12" s="176" t="str">
+      <c r="M12" s="175" t="str">
         <f t="shared" si="1"/>
         <v>Expect3</v>
       </c>
-      <c r="N12" s="176" t="str">
+      <c r="N12" s="175" t="str">
         <f t="shared" ref="N12:O12" si="2">"Expect"&amp;N11</f>
         <v>Expect4</v>
       </c>
-      <c r="O12" s="176" t="str">
+      <c r="O12" s="175" t="str">
         <f t="shared" si="2"/>
         <v>Expect5</v>
       </c>
-      <c r="P12" s="176" t="str">
+      <c r="P12" s="175" t="str">
         <f t="shared" ref="P12:Q12" si="3">"Expect"&amp;P11</f>
         <v>Expect6</v>
       </c>
-      <c r="Q12" s="176" t="str">
+      <c r="Q12" s="175" t="str">
         <f t="shared" si="3"/>
         <v>Expect7</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="165" customFormat="1">
-      <c r="A13" s="162">
+    <row r="13" spans="1:17" s="164" customFormat="1">
+      <c r="A13" s="161">
         <v>1</v>
       </c>
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="209" t="s">
+      <c r="C13" s="163"/>
+      <c r="D13" s="210" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="210"/>
-      <c r="F13" s="210"/>
-      <c r="G13" s="210"/>
-      <c r="H13" s="210"/>
+      <c r="E13" s="211"/>
+      <c r="F13" s="211"/>
+      <c r="G13" s="211"/>
+      <c r="H13" s="211"/>
       <c r="I13" s="212"/>
-      <c r="J13" s="211" t="s">
+      <c r="J13" s="202" t="s">
         <v>120</v>
       </c>
-      <c r="K13" s="207" t="s">
+      <c r="K13" s="208" t="s">
         <v>92</v>
       </c>
-      <c r="L13" s="208"/>
-      <c r="M13" s="208"/>
-      <c r="N13" s="208" t="s">
+      <c r="L13" s="209"/>
+      <c r="M13" s="209"/>
+      <c r="N13" s="209" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="208"/>
-      <c r="P13" s="195" t="s">
+      <c r="O13" s="209"/>
+      <c r="P13" s="194" t="s">
         <v>125</v>
       </c>
-      <c r="Q13" s="195" t="s">
+      <c r="Q13" s="194" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="165" customFormat="1">
-      <c r="A14" s="162">
+    <row r="14" spans="1:17" s="164" customFormat="1">
+      <c r="A14" s="161">
         <f>A13+1</f>
         <v>2</v>
       </c>
-      <c r="B14" s="163" t="s">
+      <c r="B14" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="166"/>
-      <c r="D14" s="163" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="162" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
-      <c r="I14" s="202"/>
-      <c r="J14" s="202"/>
-      <c r="K14" s="200" t="s">
+      <c r="E14" s="193"/>
+      <c r="F14" s="193"/>
+      <c r="G14" s="193"/>
+      <c r="H14" s="193"/>
+      <c r="I14" s="201"/>
+      <c r="J14" s="201"/>
+      <c r="K14" s="199" t="s">
         <v>91</v>
       </c>
-      <c r="L14" s="193" t="s">
+      <c r="L14" s="192" t="s">
         <v>94</v>
       </c>
-      <c r="M14" s="193" t="s">
+      <c r="M14" s="192" t="s">
         <v>93</v>
       </c>
-      <c r="N14" s="192" t="s">
+      <c r="N14" s="191" t="s">
         <v>91</v>
       </c>
-      <c r="O14" s="192" t="s">
+      <c r="O14" s="191" t="s">
         <v>94</v>
       </c>
-      <c r="P14" s="192" t="s">
+      <c r="P14" s="191" t="s">
         <v>126</v>
       </c>
-      <c r="Q14" s="192"/>
-    </row>
-    <row r="15" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A15" s="162">
-        <f t="shared" ref="A15:A46" si="4">A14+1</f>
+      <c r="Q14" s="191"/>
+    </row>
+    <row r="15" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A15" s="161">
+        <f t="shared" ref="A15:A53" si="4">A14+1</f>
         <v>3</v>
       </c>
-      <c r="B15" s="163" t="s">
+      <c r="B15" s="162" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="166"/>
-      <c r="D15" s="163" t="s">
+      <c r="C15" s="165"/>
+      <c r="D15" s="162" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="163" t="s">
+      <c r="E15" s="162" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="163" t="s">
+      <c r="F15" s="162" t="s">
         <v>114</v>
       </c>
-      <c r="G15" s="163" t="s">
+      <c r="G15" s="162" t="s">
         <v>115</v>
       </c>
-      <c r="H15" s="163" t="s">
+      <c r="H15" s="162" t="s">
         <v>116</v>
       </c>
-      <c r="I15" s="201" t="s">
+      <c r="I15" s="200" t="s">
         <v>117</v>
       </c>
-      <c r="J15" s="201"/>
-      <c r="K15" s="200"/>
-      <c r="L15" s="193"/>
-      <c r="M15" s="193"/>
-      <c r="N15" s="192"/>
-      <c r="O15" s="192"/>
-      <c r="P15" s="192"/>
-      <c r="Q15" s="192"/>
-    </row>
-    <row r="16" spans="1:17" s="165" customFormat="1">
-      <c r="A16" s="162">
+      <c r="J15" s="200"/>
+      <c r="K15" s="199"/>
+      <c r="L15" s="192"/>
+      <c r="M15" s="192"/>
+      <c r="N15" s="191"/>
+      <c r="O15" s="191"/>
+      <c r="P15" s="191"/>
+      <c r="Q15" s="191"/>
+    </row>
+    <row r="16" spans="1:17" s="164" customFormat="1">
+      <c r="A16" s="161">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B16" s="167" t="s">
+      <c r="B16" s="166" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="168"/>
-      <c r="D16" s="168"/>
-      <c r="E16" s="168"/>
-      <c r="F16" s="168"/>
-      <c r="G16" s="168"/>
-      <c r="H16" s="168"/>
-      <c r="I16" s="168"/>
-      <c r="J16" s="213" t="s">
+      <c r="C16" s="167"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="203" t="s">
         <v>121</v>
       </c>
-      <c r="K16" s="188" t="s">
+      <c r="K16" s="187" t="s">
         <v>96</v>
       </c>
-      <c r="L16" s="189" t="s">
+      <c r="L16" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="M16" s="189" t="s">
+      <c r="M16" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="N16" s="190" t="s">
+      <c r="N16" s="189" t="s">
         <v>83</v>
       </c>
-      <c r="O16" s="191" t="s">
+      <c r="O16" s="190" t="s">
         <v>83</v>
       </c>
-      <c r="P16" s="191" t="s">
+      <c r="P16" s="190" t="s">
         <v>127</v>
       </c>
-      <c r="Q16" s="191" t="s">
+      <c r="Q16" s="190" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="165" customFormat="1">
-      <c r="A17" s="162">
+    <row r="17" spans="1:17" s="164" customFormat="1">
+      <c r="A17" s="161">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B17" s="161" t="s">
+      <c r="B17" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="164">
+      <c r="C17" s="163">
         <v>1</v>
       </c>
-      <c r="D17" s="178" t="s">
+      <c r="D17" s="177" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="178">
+      <c r="E17" s="177">
         <v>10</v>
       </c>
-      <c r="F17" s="178">
+      <c r="F17" s="177">
         <v>20</v>
       </c>
-      <c r="G17" s="178">
+      <c r="G17" s="177">
         <v>30</v>
       </c>
-      <c r="H17" s="178">
+      <c r="H17" s="177">
         <v>40</v>
       </c>
-      <c r="I17" s="178" t="s">
+      <c r="I17" s="177" t="s">
         <v>108</v>
       </c>
-      <c r="J17" s="178" t="s">
+      <c r="J17" s="177" t="s">
         <v>122</v>
       </c>
-      <c r="K17" s="185" t="s">
+      <c r="K17" s="184" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="185" t="s">
+      <c r="L17" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="M17" s="185">
+      <c r="M17" s="184">
         <v>1</v>
       </c>
-      <c r="N17" s="185">
+      <c r="N17" s="184">
         <v>1</v>
       </c>
-      <c r="O17" s="185" t="s">
+      <c r="O17" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="P17" s="185" t="s">
+      <c r="P17" s="184" t="s">
         <v>122</v>
       </c>
-      <c r="Q17" s="185" t="s">
+      <c r="Q17" s="184" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="162">
+      <c r="A18" s="161">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="B18" s="161" t="s">
+      <c r="B18" s="160" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="178">
+      <c r="E18" s="177">
         <v>10</v>
       </c>
-      <c r="F18" s="178">
+      <c r="F18" s="177">
         <v>20</v>
       </c>
-      <c r="G18" s="178">
+      <c r="G18" s="177">
         <v>30</v>
       </c>
-      <c r="H18" s="178">
+      <c r="H18" s="177">
         <v>40</v>
       </c>
       <c r="I18" s="79" t="s">
         <v>109</v>
       </c>
       <c r="J18" s="79"/>
-      <c r="K18" s="186"/>
-      <c r="L18" s="194" t="s">
+      <c r="K18" s="185"/>
+      <c r="L18" s="193" t="s">
         <v>98</v>
       </c>
-      <c r="M18" s="194"/>
-      <c r="N18" s="194"/>
-      <c r="O18" s="194" t="s">
+      <c r="M18" s="193"/>
+      <c r="N18" s="193"/>
+      <c r="O18" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P18" s="185" t="s">
+      <c r="P18" s="184" t="s">
         <v>123</v>
       </c>
-      <c r="Q18" s="185"/>
-    </row>
-    <row r="19" spans="1:17" s="165" customFormat="1">
-      <c r="A19" s="162">
+      <c r="Q18" s="184"/>
+    </row>
+    <row r="19" spans="1:17" s="164" customFormat="1">
+      <c r="A19" s="161">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="B19" s="161" t="s">
+      <c r="B19" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="166"/>
+      <c r="C19" s="165"/>
       <c r="D19" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="178">
+      <c r="E19" s="177">
         <v>10</v>
       </c>
-      <c r="F19" s="178">
+      <c r="F19" s="177">
         <v>20</v>
       </c>
-      <c r="G19" s="178">
+      <c r="G19" s="177">
         <v>30</v>
       </c>
-      <c r="H19" s="178">
+      <c r="H19" s="177">
         <v>40</v>
       </c>
       <c r="I19" s="79" t="s">
         <v>118</v>
       </c>
       <c r="J19" s="79"/>
-      <c r="K19" s="187"/>
-      <c r="L19" s="187" t="s">
+      <c r="K19" s="186"/>
+      <c r="L19" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="M19" s="187"/>
-      <c r="N19" s="187"/>
-      <c r="O19" s="187" t="s">
+      <c r="M19" s="186"/>
+      <c r="N19" s="186"/>
+      <c r="O19" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="P19" s="187" t="s">
+      <c r="P19" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="Q19" s="187"/>
-    </row>
-    <row r="20" spans="1:17" s="165" customFormat="1">
-      <c r="A20" s="162">
+      <c r="Q19" s="186"/>
+    </row>
+    <row r="20" spans="1:17" s="164" customFormat="1">
+      <c r="A20" s="161">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="B20" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="166"/>
+      <c r="C20" s="165"/>
       <c r="D20" s="79" t="s">
         <v>87</v>
       </c>
@@ -6393,25 +6412,25 @@
       <c r="H20" s="79"/>
       <c r="I20" s="79"/>
       <c r="J20" s="79"/>
-      <c r="K20" s="170"/>
+      <c r="K20" s="169"/>
       <c r="L20" s="79"/>
       <c r="M20" s="79"/>
-      <c r="N20" s="179">
+      <c r="N20" s="178">
         <v>2</v>
       </c>
-      <c r="O20" s="180"/>
-      <c r="P20" s="180"/>
-      <c r="Q20" s="180"/>
-    </row>
-    <row r="21" spans="1:17" s="165" customFormat="1">
-      <c r="A21" s="162">
+      <c r="O20" s="179"/>
+      <c r="P20" s="179"/>
+      <c r="Q20" s="179"/>
+    </row>
+    <row r="21" spans="1:17" s="164" customFormat="1">
+      <c r="A21" s="161">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="B21" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="166"/>
+      <c r="C21" s="165"/>
       <c r="D21" s="79"/>
       <c r="E21" s="79"/>
       <c r="F21" s="79"/>
@@ -6419,25 +6438,25 @@
       <c r="H21" s="79"/>
       <c r="I21" s="79"/>
       <c r="J21" s="79"/>
-      <c r="K21" s="171"/>
-      <c r="L21" s="169"/>
-      <c r="M21" s="169"/>
-      <c r="N21" s="177"/>
-      <c r="O21" s="178" t="s">
+      <c r="K21" s="170"/>
+      <c r="L21" s="168"/>
+      <c r="M21" s="168"/>
+      <c r="N21" s="176"/>
+      <c r="O21" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P21" s="178"/>
-      <c r="Q21" s="178"/>
-    </row>
-    <row r="22" spans="1:17" s="165" customFormat="1">
-      <c r="A22" s="162">
+      <c r="P21" s="177"/>
+      <c r="Q21" s="177"/>
+    </row>
+    <row r="22" spans="1:17" s="164" customFormat="1">
+      <c r="A22" s="161">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="B22" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="166"/>
+      <c r="C22" s="165"/>
       <c r="D22" s="79"/>
       <c r="E22" s="79"/>
       <c r="F22" s="79"/>
@@ -6445,25 +6464,25 @@
       <c r="H22" s="79"/>
       <c r="I22" s="79"/>
       <c r="J22" s="79"/>
-      <c r="K22" s="170"/>
+      <c r="K22" s="169"/>
       <c r="L22" s="79"/>
       <c r="M22" s="79"/>
-      <c r="N22" s="179"/>
-      <c r="O22" s="180" t="s">
+      <c r="N22" s="178"/>
+      <c r="O22" s="179" t="s">
         <v>87</v>
       </c>
-      <c r="P22" s="180"/>
-      <c r="Q22" s="180"/>
-    </row>
-    <row r="23" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A23" s="162">
+      <c r="P22" s="179"/>
+      <c r="Q22" s="179"/>
+    </row>
+    <row r="23" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A23" s="161">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="B23" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="166"/>
+      <c r="C23" s="165"/>
       <c r="D23" s="79"/>
       <c r="E23" s="79"/>
       <c r="F23" s="79"/>
@@ -6471,27 +6490,27 @@
       <c r="H23" s="79"/>
       <c r="I23" s="79"/>
       <c r="J23" s="79"/>
-      <c r="K23" s="172"/>
-      <c r="L23" s="181"/>
-      <c r="M23" s="182"/>
-      <c r="N23" s="183">
+      <c r="K23" s="171"/>
+      <c r="L23" s="180"/>
+      <c r="M23" s="181"/>
+      <c r="N23" s="182">
         <v>3</v>
       </c>
-      <c r="O23" s="178" t="s">
+      <c r="O23" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P23" s="184"/>
-      <c r="Q23" s="184"/>
-    </row>
-    <row r="24" spans="1:17" s="165" customFormat="1">
-      <c r="A24" s="162">
+      <c r="P23" s="183"/>
+      <c r="Q23" s="183"/>
+    </row>
+    <row r="24" spans="1:17" s="164" customFormat="1">
+      <c r="A24" s="161">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="B24" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="166"/>
+      <c r="C24" s="165"/>
       <c r="D24" s="79"/>
       <c r="E24" s="79"/>
       <c r="F24" s="79"/>
@@ -6499,27 +6518,27 @@
       <c r="H24" s="79"/>
       <c r="I24" s="79"/>
       <c r="J24" s="79"/>
-      <c r="K24" s="171"/>
-      <c r="L24" s="169"/>
-      <c r="M24" s="169"/>
-      <c r="N24" s="177" t="s">
+      <c r="K24" s="170"/>
+      <c r="L24" s="168"/>
+      <c r="M24" s="168"/>
+      <c r="N24" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="O24" s="178" t="s">
+      <c r="O24" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P24" s="178"/>
-      <c r="Q24" s="178"/>
-    </row>
-    <row r="25" spans="1:17" s="165" customFormat="1">
-      <c r="A25" s="162">
+      <c r="P24" s="177"/>
+      <c r="Q24" s="177"/>
+    </row>
+    <row r="25" spans="1:17" s="164" customFormat="1">
+      <c r="A25" s="161">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="B25" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="166"/>
+      <c r="C25" s="165"/>
       <c r="D25" s="79"/>
       <c r="E25" s="79"/>
       <c r="F25" s="79"/>
@@ -6527,25 +6546,25 @@
       <c r="H25" s="79"/>
       <c r="I25" s="79"/>
       <c r="J25" s="79"/>
-      <c r="K25" s="170"/>
+      <c r="K25" s="169"/>
       <c r="L25" s="79"/>
       <c r="M25" s="79"/>
-      <c r="N25" s="179"/>
-      <c r="O25" s="178" t="s">
+      <c r="N25" s="178"/>
+      <c r="O25" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P25" s="180"/>
-      <c r="Q25" s="180"/>
-    </row>
-    <row r="26" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A26" s="162">
+      <c r="P25" s="179"/>
+      <c r="Q25" s="179"/>
+    </row>
+    <row r="26" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A26" s="161">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="B26" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="166"/>
+      <c r="C26" s="165"/>
       <c r="D26" s="79"/>
       <c r="E26" s="79"/>
       <c r="F26" s="79"/>
@@ -6553,25 +6572,25 @@
       <c r="H26" s="79"/>
       <c r="I26" s="79"/>
       <c r="J26" s="79"/>
-      <c r="K26" s="172"/>
-      <c r="L26" s="181"/>
-      <c r="M26" s="182"/>
-      <c r="N26" s="183"/>
-      <c r="O26" s="178" t="s">
+      <c r="K26" s="171"/>
+      <c r="L26" s="180"/>
+      <c r="M26" s="181"/>
+      <c r="N26" s="182"/>
+      <c r="O26" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P26" s="184"/>
-      <c r="Q26" s="184"/>
-    </row>
-    <row r="27" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A27" s="162">
+      <c r="P26" s="183"/>
+      <c r="Q26" s="183"/>
+    </row>
+    <row r="27" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A27" s="161">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
       <c r="B27" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="166"/>
+      <c r="C27" s="165"/>
       <c r="D27" s="79"/>
       <c r="E27" s="79"/>
       <c r="F27" s="79"/>
@@ -6579,160 +6598,160 @@
       <c r="H27" s="79"/>
       <c r="I27" s="79"/>
       <c r="J27" s="79"/>
-      <c r="K27" s="171"/>
-      <c r="L27" s="169"/>
-      <c r="M27" s="169"/>
-      <c r="N27" s="177"/>
-      <c r="O27" s="178" t="s">
+      <c r="K27" s="170"/>
+      <c r="L27" s="168"/>
+      <c r="M27" s="168"/>
+      <c r="N27" s="176"/>
+      <c r="O27" s="177" t="s">
         <v>84</v>
       </c>
-      <c r="P27" s="178"/>
-      <c r="Q27" s="178"/>
-    </row>
-    <row r="28" spans="1:17" s="165" customFormat="1">
-      <c r="A28" s="162">
+      <c r="P27" s="177"/>
+      <c r="Q27" s="177"/>
+    </row>
+    <row r="28" spans="1:17" s="164" customFormat="1">
+      <c r="A28" s="161">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="B28" s="167" t="s">
+      <c r="B28" s="166" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="168"/>
-      <c r="D28" s="168"/>
-      <c r="E28" s="168"/>
-      <c r="F28" s="168"/>
-      <c r="G28" s="168"/>
-      <c r="H28" s="168"/>
-      <c r="I28" s="168"/>
-      <c r="J28" s="213" t="s">
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
+      <c r="H28" s="167"/>
+      <c r="I28" s="167"/>
+      <c r="J28" s="203" t="s">
         <v>121</v>
       </c>
-      <c r="K28" s="188" t="s">
+      <c r="K28" s="187" t="s">
         <v>96</v>
       </c>
-      <c r="L28" s="189" t="s">
+      <c r="L28" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="M28" s="189" t="s">
+      <c r="M28" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="N28" s="190" t="s">
+      <c r="N28" s="189" t="s">
         <v>83</v>
       </c>
-      <c r="O28" s="191" t="s">
+      <c r="O28" s="190" t="s">
         <v>83</v>
       </c>
-      <c r="P28" s="191" t="s">
+      <c r="P28" s="190" t="s">
         <v>127</v>
       </c>
-      <c r="Q28" s="191" t="s">
+      <c r="Q28" s="190" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="165" customFormat="1">
-      <c r="A29" s="162">
+    <row r="29" spans="1:17" s="164" customFormat="1">
+      <c r="A29" s="161">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="B29" s="161" t="s">
+      <c r="B29" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="164">
+      <c r="C29" s="163">
         <v>2</v>
       </c>
-      <c r="D29" s="178" t="s">
+      <c r="D29" s="177" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="178">
+      <c r="E29" s="177">
         <v>10</v>
       </c>
-      <c r="F29" s="178">
+      <c r="F29" s="177">
         <v>20</v>
       </c>
-      <c r="G29" s="178">
+      <c r="G29" s="177">
         <v>30</v>
       </c>
-      <c r="H29" s="178">
+      <c r="H29" s="177">
         <v>40</v>
       </c>
-      <c r="I29" s="178" t="s">
+      <c r="I29" s="177" t="s">
         <v>108</v>
       </c>
-      <c r="J29" s="178" t="s">
+      <c r="J29" s="177" t="s">
         <v>123</v>
       </c>
-      <c r="K29" s="185" t="s">
+      <c r="K29" s="184" t="s">
         <v>86</v>
       </c>
-      <c r="L29" s="185" t="s">
+      <c r="L29" s="184" t="s">
         <v>103</v>
       </c>
-      <c r="M29" s="185">
+      <c r="M29" s="184">
         <v>1</v>
       </c>
-      <c r="N29" s="185">
+      <c r="N29" s="184">
         <v>1</v>
       </c>
-      <c r="O29" s="185" t="s">
+      <c r="O29" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="P29" s="185" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q29" s="185" t="s">
+      <c r="P29" s="184" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q29" s="184" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:17">
-      <c r="A30" s="162">
+      <c r="A30" s="161">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="B30" s="161" t="s">
+      <c r="B30" s="160" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="178">
+      <c r="E30" s="177">
         <v>10</v>
       </c>
-      <c r="F30" s="178">
+      <c r="F30" s="177">
         <v>20</v>
       </c>
-      <c r="G30" s="178">
+      <c r="G30" s="177">
         <v>30</v>
       </c>
-      <c r="H30" s="178">
+      <c r="H30" s="177">
         <v>40</v>
       </c>
       <c r="I30" s="79" t="s">
         <v>109</v>
       </c>
       <c r="J30" s="79"/>
-      <c r="K30" s="186"/>
-      <c r="L30" s="194" t="s">
+      <c r="K30" s="185"/>
+      <c r="L30" s="193" t="s">
         <v>106</v>
       </c>
-      <c r="M30" s="194"/>
-      <c r="N30" s="194"/>
-      <c r="O30" s="194" t="s">
+      <c r="M30" s="193"/>
+      <c r="N30" s="193"/>
+      <c r="O30" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P30" s="185" t="s">
+      <c r="P30" s="184" t="s">
         <v>87</v>
       </c>
-      <c r="Q30" s="185"/>
-    </row>
-    <row r="31" spans="1:17" s="165" customFormat="1">
-      <c r="A31" s="162">
+      <c r="Q30" s="184"/>
+    </row>
+    <row r="31" spans="1:17" s="164" customFormat="1">
+      <c r="A31" s="161">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="B31" s="161" t="s">
+      <c r="B31" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="166"/>
+      <c r="C31" s="165"/>
       <c r="D31" s="79" t="s">
         <v>87</v>
       </c>
@@ -6742,27 +6761,27 @@
       <c r="H31" s="79"/>
       <c r="I31" s="79"/>
       <c r="J31" s="79"/>
-      <c r="K31" s="187"/>
-      <c r="L31" s="187" t="s">
+      <c r="K31" s="186"/>
+      <c r="L31" s="186" t="s">
         <v>107</v>
       </c>
-      <c r="M31" s="187"/>
-      <c r="N31" s="187"/>
-      <c r="O31" s="187" t="s">
+      <c r="M31" s="186"/>
+      <c r="N31" s="186"/>
+      <c r="O31" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="P31" s="187"/>
-      <c r="Q31" s="187"/>
-    </row>
-    <row r="32" spans="1:17" s="165" customFormat="1">
-      <c r="A32" s="162">
+      <c r="P31" s="186"/>
+      <c r="Q31" s="186"/>
+    </row>
+    <row r="32" spans="1:17" s="164" customFormat="1">
+      <c r="A32" s="161">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="B32" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="166"/>
+      <c r="C32" s="165"/>
       <c r="D32" s="79"/>
       <c r="E32" s="79"/>
       <c r="F32" s="79"/>
@@ -6770,27 +6789,27 @@
       <c r="H32" s="79"/>
       <c r="I32" s="79"/>
       <c r="J32" s="79"/>
-      <c r="K32" s="170"/>
+      <c r="K32" s="169"/>
       <c r="L32" s="79" t="s">
         <v>87</v>
       </c>
       <c r="M32" s="79"/>
-      <c r="N32" s="179">
+      <c r="N32" s="178">
         <v>2</v>
       </c>
-      <c r="O32" s="180"/>
-      <c r="P32" s="180"/>
-      <c r="Q32" s="180"/>
-    </row>
-    <row r="33" spans="1:17" s="165" customFormat="1">
-      <c r="A33" s="162">
+      <c r="O32" s="179"/>
+      <c r="P32" s="179"/>
+      <c r="Q32" s="179"/>
+    </row>
+    <row r="33" spans="1:17" s="164" customFormat="1">
+      <c r="A33" s="161">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="B33" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="166"/>
+      <c r="C33" s="165"/>
       <c r="D33" s="79"/>
       <c r="E33" s="79"/>
       <c r="F33" s="79"/>
@@ -6798,27 +6817,27 @@
       <c r="H33" s="79"/>
       <c r="I33" s="79"/>
       <c r="J33" s="79"/>
-      <c r="K33" s="171"/>
-      <c r="L33" s="169"/>
-      <c r="M33" s="169"/>
-      <c r="N33" s="177" t="s">
+      <c r="K33" s="170"/>
+      <c r="L33" s="168"/>
+      <c r="M33" s="168"/>
+      <c r="N33" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="O33" s="178" t="s">
+      <c r="O33" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P33" s="178"/>
-      <c r="Q33" s="178"/>
-    </row>
-    <row r="34" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A34" s="162">
+      <c r="P33" s="177"/>
+      <c r="Q33" s="177"/>
+    </row>
+    <row r="34" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A34" s="161">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="B34" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="166"/>
+      <c r="C34" s="165"/>
       <c r="D34" s="79"/>
       <c r="E34" s="79"/>
       <c r="F34" s="79"/>
@@ -6826,240 +6845,240 @@
       <c r="H34" s="79"/>
       <c r="I34" s="79"/>
       <c r="J34" s="79"/>
-      <c r="K34" s="170"/>
+      <c r="K34" s="169"/>
       <c r="L34" s="79"/>
       <c r="M34" s="79"/>
-      <c r="N34" s="179"/>
-      <c r="O34" s="180" t="s">
+      <c r="N34" s="178"/>
+      <c r="O34" s="179" t="s">
         <v>87</v>
       </c>
-      <c r="P34" s="180"/>
-      <c r="Q34" s="180"/>
-    </row>
-    <row r="35" spans="1:17" s="165" customFormat="1">
-      <c r="A35" s="162">
+      <c r="P34" s="179"/>
+      <c r="Q34" s="179"/>
+    </row>
+    <row r="35" spans="1:17" s="164" customFormat="1">
+      <c r="A35" s="161">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="B35" s="167" t="s">
+      <c r="B35" s="166" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="168"/>
-      <c r="D35" s="168"/>
-      <c r="E35" s="168"/>
-      <c r="F35" s="168"/>
-      <c r="G35" s="168"/>
-      <c r="H35" s="168"/>
-      <c r="I35" s="168"/>
-      <c r="J35" s="213" t="s">
+      <c r="C35" s="167"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="167"/>
+      <c r="I35" s="167"/>
+      <c r="J35" s="203" t="s">
         <v>121</v>
       </c>
-      <c r="K35" s="188" t="s">
+      <c r="K35" s="187" t="s">
         <v>96</v>
       </c>
-      <c r="L35" s="189" t="s">
+      <c r="L35" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="M35" s="189" t="s">
+      <c r="M35" s="188" t="s">
         <v>83</v>
       </c>
-      <c r="N35" s="190" t="s">
+      <c r="N35" s="189" t="s">
         <v>83</v>
       </c>
-      <c r="O35" s="191" t="s">
+      <c r="O35" s="190" t="s">
         <v>83</v>
       </c>
-      <c r="P35" s="191" t="s">
+      <c r="P35" s="190" t="s">
         <v>127</v>
       </c>
-      <c r="Q35" s="191" t="s">
+      <c r="Q35" s="190" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="165" customFormat="1">
-      <c r="A36" s="162">
+    <row r="36" spans="1:17" s="164" customFormat="1">
+      <c r="A36" s="161">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="B36" s="161" t="s">
+      <c r="B36" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="164">
+      <c r="C36" s="163">
         <v>3</v>
       </c>
-      <c r="D36" s="178" t="s">
+      <c r="D36" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="178">
+      <c r="E36" s="177">
         <v>10</v>
       </c>
-      <c r="F36" s="178">
+      <c r="F36" s="177">
         <v>20</v>
       </c>
-      <c r="G36" s="178">
+      <c r="G36" s="177">
         <v>30</v>
       </c>
-      <c r="H36" s="178">
+      <c r="H36" s="177">
         <v>40</v>
       </c>
-      <c r="I36" s="178" t="s">
+      <c r="I36" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="J36" s="178" t="s">
+      <c r="J36" s="177" t="s">
         <v>124</v>
       </c>
-      <c r="K36" s="185" t="s">
+      <c r="K36" s="184" t="s">
         <v>86</v>
       </c>
-      <c r="L36" s="185" t="s">
+      <c r="L36" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="M36" s="185">
+      <c r="M36" s="184">
         <v>1</v>
       </c>
-      <c r="N36" s="185">
+      <c r="N36" s="184">
         <v>1</v>
       </c>
-      <c r="O36" s="185" t="s">
+      <c r="O36" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="P36" s="185" t="s">
+      <c r="P36" s="184" t="s">
         <v>123</v>
       </c>
-      <c r="Q36" s="185" t="s">
+      <c r="Q36" s="184" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="162">
+      <c r="A37" s="161">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="B37" s="161" t="s">
+      <c r="B37" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="178" t="s">
+      <c r="D37" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="E37" s="178">
+      <c r="E37" s="177">
         <v>10</v>
       </c>
-      <c r="F37" s="178">
+      <c r="F37" s="177">
         <v>20</v>
       </c>
-      <c r="G37" s="178">
+      <c r="G37" s="177">
         <v>30</v>
       </c>
-      <c r="H37" s="178">
+      <c r="H37" s="177">
         <v>40</v>
       </c>
-      <c r="I37" s="178" t="s">
+      <c r="I37" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="J37" s="178"/>
-      <c r="K37" s="186"/>
-      <c r="L37" s="194" t="s">
+      <c r="J37" s="177"/>
+      <c r="K37" s="185"/>
+      <c r="L37" s="193" t="s">
         <v>98</v>
       </c>
-      <c r="M37" s="194"/>
-      <c r="N37" s="194"/>
-      <c r="O37" s="194" t="s">
+      <c r="M37" s="193"/>
+      <c r="N37" s="193"/>
+      <c r="O37" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P37" s="185" t="s">
+      <c r="P37" s="184" t="s">
         <v>124</v>
       </c>
-      <c r="Q37" s="185"/>
-    </row>
-    <row r="38" spans="1:17" s="165" customFormat="1">
-      <c r="A38" s="162">
+      <c r="Q37" s="184"/>
+    </row>
+    <row r="38" spans="1:17" s="164" customFormat="1">
+      <c r="A38" s="161">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="B38" s="161" t="s">
+      <c r="B38" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="166"/>
-      <c r="D38" s="178" t="s">
+      <c r="C38" s="165"/>
+      <c r="D38" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="178">
+      <c r="E38" s="177">
         <v>10</v>
       </c>
-      <c r="F38" s="178">
+      <c r="F38" s="177">
         <v>20</v>
       </c>
-      <c r="G38" s="178">
+      <c r="G38" s="177">
         <v>30</v>
       </c>
-      <c r="H38" s="178">
+      <c r="H38" s="177">
         <v>40</v>
       </c>
-      <c r="I38" s="178" t="s">
+      <c r="I38" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="J38" s="178"/>
-      <c r="K38" s="187"/>
-      <c r="L38" s="187" t="s">
+      <c r="J38" s="177"/>
+      <c r="K38" s="186"/>
+      <c r="L38" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="M38" s="187"/>
-      <c r="N38" s="187"/>
-      <c r="O38" s="187" t="s">
+      <c r="M38" s="186"/>
+      <c r="N38" s="186"/>
+      <c r="O38" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="P38" s="187" t="s">
+      <c r="P38" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="Q38" s="187"/>
-    </row>
-    <row r="39" spans="1:17" s="165" customFormat="1">
-      <c r="A39" s="162">
+      <c r="Q38" s="186"/>
+    </row>
+    <row r="39" spans="1:17" s="164" customFormat="1">
+      <c r="A39" s="161">
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="B39" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="166"/>
-      <c r="D39" s="178" t="s">
+      <c r="C39" s="165"/>
+      <c r="D39" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="178">
+      <c r="E39" s="177">
         <v>10</v>
       </c>
-      <c r="F39" s="178">
+      <c r="F39" s="177">
         <v>20</v>
       </c>
-      <c r="G39" s="178">
+      <c r="G39" s="177">
         <v>30</v>
       </c>
-      <c r="H39" s="178">
+      <c r="H39" s="177">
         <v>40</v>
       </c>
-      <c r="I39" s="178" t="s">
+      <c r="I39" s="177" t="s">
         <v>110</v>
       </c>
-      <c r="J39" s="178"/>
-      <c r="K39" s="170"/>
+      <c r="J39" s="177"/>
+      <c r="K39" s="169"/>
       <c r="L39" s="79"/>
       <c r="M39" s="79"/>
-      <c r="N39" s="179">
+      <c r="N39" s="178">
         <v>2</v>
       </c>
-      <c r="O39" s="180"/>
-      <c r="P39" s="180"/>
-      <c r="Q39" s="180"/>
-    </row>
-    <row r="40" spans="1:17" s="165" customFormat="1">
-      <c r="A40" s="162">
+      <c r="O39" s="179"/>
+      <c r="P39" s="179"/>
+      <c r="Q39" s="179"/>
+    </row>
+    <row r="40" spans="1:17" s="164" customFormat="1">
+      <c r="A40" s="161">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="B40" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="166"/>
+      <c r="C40" s="165"/>
       <c r="D40" s="79" t="s">
         <v>87</v>
       </c>
@@ -7069,25 +7088,25 @@
       <c r="H40" s="79"/>
       <c r="I40" s="79"/>
       <c r="J40" s="79"/>
-      <c r="K40" s="171"/>
-      <c r="L40" s="169"/>
-      <c r="M40" s="169"/>
-      <c r="N40" s="177"/>
-      <c r="O40" s="178" t="s">
+      <c r="K40" s="170"/>
+      <c r="L40" s="168"/>
+      <c r="M40" s="168"/>
+      <c r="N40" s="176"/>
+      <c r="O40" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P40" s="178"/>
-      <c r="Q40" s="178"/>
-    </row>
-    <row r="41" spans="1:17" s="165" customFormat="1">
-      <c r="A41" s="162">
+      <c r="P40" s="177"/>
+      <c r="Q40" s="177"/>
+    </row>
+    <row r="41" spans="1:17" s="164" customFormat="1">
+      <c r="A41" s="161">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="B41" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="166"/>
+      <c r="C41" s="165"/>
       <c r="D41" s="79"/>
       <c r="E41" s="79"/>
       <c r="F41" s="79"/>
@@ -7095,25 +7114,25 @@
       <c r="H41" s="79"/>
       <c r="I41" s="79"/>
       <c r="J41" s="79"/>
-      <c r="K41" s="170"/>
+      <c r="K41" s="169"/>
       <c r="L41" s="79"/>
       <c r="M41" s="79"/>
-      <c r="N41" s="179"/>
-      <c r="O41" s="180" t="s">
+      <c r="N41" s="178"/>
+      <c r="O41" s="179" t="s">
         <v>87</v>
       </c>
-      <c r="P41" s="180"/>
-      <c r="Q41" s="180"/>
-    </row>
-    <row r="42" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A42" s="162">
+      <c r="P41" s="179"/>
+      <c r="Q41" s="179"/>
+    </row>
+    <row r="42" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A42" s="161">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="B42" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="166"/>
+      <c r="C42" s="165"/>
       <c r="D42" s="79"/>
       <c r="E42" s="79"/>
       <c r="F42" s="79"/>
@@ -7121,27 +7140,27 @@
       <c r="H42" s="79"/>
       <c r="I42" s="79"/>
       <c r="J42" s="79"/>
-      <c r="K42" s="172"/>
-      <c r="L42" s="181"/>
-      <c r="M42" s="182"/>
-      <c r="N42" s="183">
+      <c r="K42" s="171"/>
+      <c r="L42" s="180"/>
+      <c r="M42" s="181"/>
+      <c r="N42" s="182">
         <v>3</v>
       </c>
-      <c r="O42" s="178" t="s">
+      <c r="O42" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P42" s="184"/>
-      <c r="Q42" s="184"/>
-    </row>
-    <row r="43" spans="1:17" s="165" customFormat="1">
-      <c r="A43" s="162">
+      <c r="P42" s="183"/>
+      <c r="Q42" s="183"/>
+    </row>
+    <row r="43" spans="1:17" s="164" customFormat="1">
+      <c r="A43" s="161">
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="B43" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="166"/>
+      <c r="C43" s="165"/>
       <c r="D43" s="79"/>
       <c r="E43" s="79"/>
       <c r="F43" s="79"/>
@@ -7149,27 +7168,27 @@
       <c r="H43" s="79"/>
       <c r="I43" s="79"/>
       <c r="J43" s="79"/>
-      <c r="K43" s="171"/>
-      <c r="L43" s="169"/>
-      <c r="M43" s="169"/>
-      <c r="N43" s="177" t="s">
+      <c r="K43" s="170"/>
+      <c r="L43" s="168"/>
+      <c r="M43" s="168"/>
+      <c r="N43" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="O43" s="178" t="s">
+      <c r="O43" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P43" s="178"/>
-      <c r="Q43" s="178"/>
-    </row>
-    <row r="44" spans="1:17" s="165" customFormat="1">
-      <c r="A44" s="162">
+      <c r="P43" s="177"/>
+      <c r="Q43" s="177"/>
+    </row>
+    <row r="44" spans="1:17" s="164" customFormat="1">
+      <c r="A44" s="161">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="B44" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="166"/>
+      <c r="C44" s="165"/>
       <c r="D44" s="79"/>
       <c r="E44" s="79"/>
       <c r="F44" s="79"/>
@@ -7177,25 +7196,25 @@
       <c r="H44" s="79"/>
       <c r="I44" s="79"/>
       <c r="J44" s="79"/>
-      <c r="K44" s="170"/>
+      <c r="K44" s="169"/>
       <c r="L44" s="79"/>
       <c r="M44" s="79"/>
-      <c r="N44" s="179"/>
-      <c r="O44" s="178" t="s">
+      <c r="N44" s="178"/>
+      <c r="O44" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P44" s="180"/>
-      <c r="Q44" s="180"/>
-    </row>
-    <row r="45" spans="1:17" s="165" customFormat="1" ht="15" thickBot="1">
-      <c r="A45" s="162">
+      <c r="P44" s="179"/>
+      <c r="Q44" s="179"/>
+    </row>
+    <row r="45" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A45" s="161">
         <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="B45" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="166"/>
+      <c r="C45" s="165"/>
       <c r="D45" s="79"/>
       <c r="E45" s="79"/>
       <c r="F45" s="79"/>
@@ -7203,25 +7222,25 @@
       <c r="H45" s="79"/>
       <c r="I45" s="79"/>
       <c r="J45" s="79"/>
-      <c r="K45" s="172"/>
-      <c r="L45" s="181"/>
-      <c r="M45" s="182"/>
-      <c r="N45" s="183"/>
-      <c r="O45" s="178" t="s">
+      <c r="K45" s="171"/>
+      <c r="L45" s="180"/>
+      <c r="M45" s="181"/>
+      <c r="N45" s="182"/>
+      <c r="O45" s="177" t="s">
         <v>101</v>
       </c>
-      <c r="P45" s="184"/>
-      <c r="Q45" s="184"/>
-    </row>
-    <row r="46" spans="1:17" s="165" customFormat="1">
-      <c r="A46" s="162">
+      <c r="P45" s="183"/>
+      <c r="Q45" s="183"/>
+    </row>
+    <row r="46" spans="1:17" s="164" customFormat="1" ht="15" thickBot="1">
+      <c r="A46" s="161">
         <f t="shared" si="4"/>
         <v>34</v>
       </c>
       <c r="B46" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="166"/>
+      <c r="C46" s="165"/>
       <c r="D46" s="79"/>
       <c r="E46" s="79"/>
       <c r="F46" s="79"/>
@@ -7229,15 +7248,258 @@
       <c r="H46" s="79"/>
       <c r="I46" s="79"/>
       <c r="J46" s="79"/>
-      <c r="K46" s="171"/>
-      <c r="L46" s="169"/>
-      <c r="M46" s="169"/>
-      <c r="N46" s="177"/>
-      <c r="O46" s="178" t="s">
+      <c r="K46" s="170"/>
+      <c r="L46" s="168"/>
+      <c r="M46" s="168"/>
+      <c r="N46" s="176"/>
+      <c r="O46" s="177" t="s">
         <v>84</v>
       </c>
-      <c r="P46" s="178"/>
-      <c r="Q46" s="178"/>
+      <c r="P46" s="177"/>
+      <c r="Q46" s="177"/>
+    </row>
+    <row r="47" spans="1:17" s="164" customFormat="1">
+      <c r="A47" s="161">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="B47" s="166" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="167"/>
+      <c r="D47" s="167"/>
+      <c r="E47" s="167"/>
+      <c r="F47" s="167"/>
+      <c r="G47" s="167"/>
+      <c r="H47" s="167"/>
+      <c r="I47" s="167"/>
+      <c r="J47" s="203" t="s">
+        <v>121</v>
+      </c>
+      <c r="K47" s="187" t="s">
+        <v>96</v>
+      </c>
+      <c r="L47" s="188" t="s">
+        <v>83</v>
+      </c>
+      <c r="M47" s="188" t="s">
+        <v>83</v>
+      </c>
+      <c r="N47" s="189" t="s">
+        <v>83</v>
+      </c>
+      <c r="O47" s="190" t="s">
+        <v>83</v>
+      </c>
+      <c r="P47" s="190" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q47" s="190" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" s="164" customFormat="1">
+      <c r="A48" s="161">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="B48" s="160" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="163">
+        <v>4</v>
+      </c>
+      <c r="D48" s="177" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" s="177">
+        <v>10</v>
+      </c>
+      <c r="F48" s="177">
+        <v>20</v>
+      </c>
+      <c r="G48" s="177">
+        <v>30</v>
+      </c>
+      <c r="H48" s="177">
+        <v>40</v>
+      </c>
+      <c r="I48" s="177" t="s">
+        <v>108</v>
+      </c>
+      <c r="J48" s="177"/>
+      <c r="K48" s="184" t="s">
+        <v>86</v>
+      </c>
+      <c r="L48" s="184" t="s">
+        <v>103</v>
+      </c>
+      <c r="M48" s="184">
+        <v>1</v>
+      </c>
+      <c r="N48" s="184">
+        <v>1</v>
+      </c>
+      <c r="O48" s="184" t="s">
+        <v>99</v>
+      </c>
+      <c r="P48" s="184" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q48" s="184" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" s="161">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="B49" s="160" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="E49" s="177">
+        <v>10</v>
+      </c>
+      <c r="F49" s="177">
+        <v>20</v>
+      </c>
+      <c r="G49" s="177">
+        <v>30</v>
+      </c>
+      <c r="H49" s="177">
+        <v>40</v>
+      </c>
+      <c r="I49" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="J49" s="79"/>
+      <c r="K49" s="185"/>
+      <c r="L49" s="193" t="s">
+        <v>106</v>
+      </c>
+      <c r="M49" s="193"/>
+      <c r="N49" s="193"/>
+      <c r="O49" s="193" t="s">
+        <v>100</v>
+      </c>
+      <c r="P49" s="184"/>
+      <c r="Q49" s="184"/>
+    </row>
+    <row r="50" spans="1:17" s="164" customFormat="1">
+      <c r="A50" s="161">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="B50" s="160" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="165"/>
+      <c r="D50" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="79"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="79"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="79"/>
+      <c r="J50" s="79"/>
+      <c r="K50" s="186"/>
+      <c r="L50" s="186" t="s">
+        <v>107</v>
+      </c>
+      <c r="M50" s="186"/>
+      <c r="N50" s="186"/>
+      <c r="O50" s="186" t="s">
+        <v>87</v>
+      </c>
+      <c r="P50" s="186"/>
+      <c r="Q50" s="186"/>
+    </row>
+    <row r="51" spans="1:17" s="164" customFormat="1">
+      <c r="A51" s="161">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="B51" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="165"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
+      <c r="K51" s="169"/>
+      <c r="L51" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="M51" s="79"/>
+      <c r="N51" s="178">
+        <v>2</v>
+      </c>
+      <c r="O51" s="179"/>
+      <c r="P51" s="179"/>
+      <c r="Q51" s="179"/>
+    </row>
+    <row r="52" spans="1:17" s="164" customFormat="1">
+      <c r="A52" s="161">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="B52" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="165"/>
+      <c r="D52" s="79"/>
+      <c r="E52" s="79"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="170"/>
+      <c r="L52" s="168"/>
+      <c r="M52" s="168"/>
+      <c r="N52" s="176" t="s">
+        <v>62</v>
+      </c>
+      <c r="O52" s="177" t="s">
+        <v>101</v>
+      </c>
+      <c r="P52" s="177"/>
+      <c r="Q52" s="177"/>
+    </row>
+    <row r="53" spans="1:17" s="164" customFormat="1">
+      <c r="A53" s="161">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="B53" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="165"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="79"/>
+      <c r="J53" s="79"/>
+      <c r="K53" s="169"/>
+      <c r="L53" s="79"/>
+      <c r="M53" s="79"/>
+      <c r="N53" s="178"/>
+      <c r="O53" s="179" t="s">
+        <v>87</v>
+      </c>
+      <c r="P53" s="179"/>
+      <c r="Q53" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
0.0.17: Support ArrayOfJson comparison type, for read array type of JSON.
</commit_message>
<xml_diff>
--- a/meta/test2/04_GetTableSample5.xlsx
+++ b/meta/test2/04_GetTableSample5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/test2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D58D757-3ACA-974B-A9B5-1C606EED4283}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7101941-F634-FF4A-BB7B-927CE746F431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11240" yWindow="2500" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="460" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="132">
   <si>
     <t>2.定義書様式に記入された情報から、メタファイルをXMLファイルに変換する処理の定義に相当するJavaソースコードが自動生成されます。</t>
   </si>
@@ -713,6 +713,14 @@
     <rPh sb="4" eb="6">
       <t xml:space="preserve">シテイ </t>
     </rPh>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>ArrayOfJson</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>jsonArray</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -5856,8 +5864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2255131-13B1-484A-9393-AFEFC966B3D8}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="G18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -6889,7 +6897,7 @@
         <v>83</v>
       </c>
       <c r="P35" s="190" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="Q35" s="190" t="s">
         <v>83</v>
@@ -6943,7 +6951,7 @@
         <v>99</v>
       </c>
       <c r="P36" s="184" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="Q36" s="184" t="s">
         <v>102</v>
@@ -6985,9 +6993,7 @@
       <c r="O37" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P37" s="184" t="s">
-        <v>124</v>
-      </c>
+      <c r="P37" s="184"/>
       <c r="Q37" s="184"/>
     </row>
     <row r="38" spans="1:17" s="164" customFormat="1">
@@ -7027,9 +7033,7 @@
       <c r="O38" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="P38" s="186" t="s">
-        <v>87</v>
-      </c>
+      <c r="P38" s="186"/>
       <c r="Q38" s="186"/>
     </row>
     <row r="39" spans="1:17" s="164" customFormat="1">

</xml_diff>

<commit_message>
0.0.18: Specify reading json file encoding with ant property option.
</commit_message>
<xml_diff>
--- a/meta/test2/04_GetTableSample5.xlsx
+++ b/meta/test2/04_GetTableSample5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestAutotest/meta/test2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7101941-F634-FF4A-BB7B-927CE746F431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736FE242-F2AA-3E4A-AA45-848DB346143B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="460" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8180" yWindow="860" windowWidth="26200" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="133">
   <si>
     <t>2.定義書様式に記入された情報から、メタファイルをXMLファイルに変換する処理の定義に相当するJavaソースコードが自動生成されます。</t>
   </si>
@@ -722,6 +722,10 @@
   <si>
     <t>jsonArray</t>
     <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>Ignore</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
@@ -5864,8 +5868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2255131-13B1-484A-9393-AFEFC966B3D8}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P49" sqref="P49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -6259,7 +6263,7 @@
         <v>83</v>
       </c>
       <c r="P16" s="190" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="Q16" s="190" t="s">
         <v>83</v>
@@ -6313,7 +6317,7 @@
         <v>99</v>
       </c>
       <c r="P17" s="184" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="Q17" s="184" t="s">
         <v>102</v>
@@ -6355,9 +6359,7 @@
       <c r="O18" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P18" s="184" t="s">
-        <v>123</v>
-      </c>
+      <c r="P18" s="184"/>
       <c r="Q18" s="184"/>
     </row>
     <row r="19" spans="1:17" s="164" customFormat="1">
@@ -6397,9 +6399,7 @@
       <c r="O19" s="186" t="s">
         <v>87</v>
       </c>
-      <c r="P19" s="186" t="s">
-        <v>87</v>
-      </c>
+      <c r="P19" s="186"/>
       <c r="Q19" s="186"/>
     </row>
     <row r="20" spans="1:17" s="164" customFormat="1">
@@ -6650,7 +6650,7 @@
         <v>83</v>
       </c>
       <c r="P28" s="190" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="Q28" s="190" t="s">
         <v>83</v>
@@ -6704,7 +6704,7 @@
         <v>99</v>
       </c>
       <c r="P29" s="184" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="Q29" s="184" t="s">
         <v>102</v>
@@ -6746,9 +6746,7 @@
       <c r="O30" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P30" s="184" t="s">
-        <v>87</v>
-      </c>
+      <c r="P30" s="184"/>
       <c r="Q30" s="184"/>
     </row>
     <row r="31" spans="1:17" s="164" customFormat="1">
@@ -6897,7 +6895,7 @@
         <v>83</v>
       </c>
       <c r="P35" s="190" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q35" s="190" t="s">
         <v>83</v>
@@ -6951,7 +6949,7 @@
         <v>99</v>
       </c>
       <c r="P36" s="184" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="Q36" s="184" t="s">
         <v>102</v>
@@ -6993,7 +6991,9 @@
       <c r="O37" s="193" t="s">
         <v>100</v>
       </c>
-      <c r="P37" s="184"/>
+      <c r="P37" s="184" t="s">
+        <v>87</v>
+      </c>
       <c r="Q37" s="184"/>
     </row>
     <row r="38" spans="1:17" s="164" customFormat="1">
@@ -7296,7 +7296,7 @@
         <v>83</v>
       </c>
       <c r="P47" s="190" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="Q47" s="190" t="s">
         <v>83</v>
@@ -7347,9 +7347,7 @@
       <c r="O48" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="P48" s="184" t="s">
-        <v>87</v>
-      </c>
+      <c r="P48" s="184"/>
       <c r="Q48" s="184" t="s">
         <v>102</v>
       </c>

</xml_diff>